<commit_message>
Inclusão de lógica para inserção do cabeçalho das planilhas
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -9,7 +9,6 @@
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="nome" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="idade" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -433,32 +432,27 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Nomes</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Idade</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Incluída a lógica de inserção de dados na planilha
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="nome" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="nomes" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,12 +443,34 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Nomes</t>
+          <t>Nome</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
           <t>Idade</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Sexo</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>carlos</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>M</t>
         </is>
       </c>
     </row>

</xml_diff>